<commit_message>
Simulation in Excel works now.
</commit_message>
<xml_diff>
--- a/ExcelYatzy/ExcelYatzy.xlsx
+++ b/ExcelYatzy/ExcelYatzy.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10305"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10305" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
-    <sheet name="SimResults" sheetId="2" r:id="rId2"/>
+    <sheet name="SimData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -351,7 +351,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -426,7 +426,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Added generation of reference data.
</commit_message>
<xml_diff>
--- a/ExcelYatzy/ExcelYatzy.xlsx
+++ b/ExcelYatzy/ExcelYatzy.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10305" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10305" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="SimData" sheetId="2" r:id="rId2"/>
+    <sheet name="RefData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -426,6 +427,21 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixing comments and adding documentation.
</commit_message>
<xml_diff>
--- a/ExcelYatzy/ExcelYatzy.xlsx
+++ b/ExcelYatzy/ExcelYatzy.xlsx
@@ -5,16 +5,15 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\strange\Documents\Visual Studio 2013\Projects\Yatzy\ExcelYatzy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\strange\documents\visual studio 2013\Projects\Yatzy\ExcelYatzy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10305" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10305"/>
   </bookViews>
   <sheets>
-    <sheet name="Overview" sheetId="1" r:id="rId1"/>
-    <sheet name="SimData" sheetId="2" r:id="rId2"/>
-    <sheet name="RefData" sheetId="3" r:id="rId3"/>
+    <sheet name="SimData" sheetId="2" r:id="rId1"/>
+    <sheet name="RefData" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -23,17 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>StDev</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -349,73 +337,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P3"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>2</v>
-      </c>
-      <c r="E1">
-        <v>3</v>
-      </c>
-      <c r="F1">
-        <v>4</v>
-      </c>
-      <c r="G1">
-        <v>5</v>
-      </c>
-      <c r="H1">
-        <v>6</v>
-      </c>
-      <c r="I1">
-        <v>7</v>
-      </c>
-      <c r="J1">
-        <v>8</v>
-      </c>
-      <c r="K1">
-        <v>9</v>
-      </c>
-      <c r="L1">
-        <v>10</v>
-      </c>
-      <c r="M1">
-        <v>11</v>
-      </c>
-      <c r="N1">
-        <v>12</v>
-      </c>
-      <c r="O1">
-        <v>13</v>
-      </c>
-      <c r="P1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -424,7 +352,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -435,19 +363,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <dataConsolidate/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>